<commit_message>
Pulling all the PlayerSheetStats stuff from the sheet and using in-game.
</commit_message>
<xml_diff>
--- a/RotoShootUnityProject/Assets/Resources/PlayerStatsSheet.xlsx
+++ b/RotoShootUnityProject/Assets/Resources/PlayerStatsSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\UnityProjects\RotoShoot\RotoShootUnityProject\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590BE14E-4957-4528-A8B3-1BE6007972F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F4ABA9-DB10-426F-87E7-1CC85FF55E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="45120" windowHeight="26136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="5868" windowWidth="28296" windowHeight="16008" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mySheet (4)" sheetId="4" r:id="rId1"/>
@@ -99,19 +99,19 @@
     <t>EnemyRateOfFireMax</t>
   </si>
   <si>
-    <t>PlayerMissileDamage</t>
+    <t>maxPlayerHP</t>
   </si>
   <si>
-    <t>StarCoinCost</t>
+    <t>playerMissileDamage</t>
   </si>
   <si>
-    <t>MAX_PLAYER_HP</t>
+    <t>powerupDuration</t>
   </si>
   <si>
-    <t>PowerupDuration</t>
+    <t>shieldDuration</t>
   </si>
   <si>
-    <t>ShieldDuration</t>
+    <t>starCoinCost</t>
   </si>
 </sst>
 </file>
@@ -678,10 +678,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -983,7 +979,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G122" sqref="G122"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,19 +998,19 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Further plumbing in of upgrades screen (item levls/costs, etc)
</commit_message>
<xml_diff>
--- a/RotoShootUnityProject/Assets/Resources/PlayerStatsSheet.xlsx
+++ b/RotoShootUnityProject/Assets/Resources/PlayerStatsSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\UnityProjects\RotoShoot\RotoShootUnityProject\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F4ABA9-DB10-426F-87E7-1CC85FF55E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7266A06E-897F-43A3-B474-238077A7EFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="5868" windowWidth="28296" windowHeight="16008" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15144" yWindow="2508" windowWidth="28296" windowHeight="21108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mySheet (4)" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>BasePlayerHP</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>starCoinCost</t>
+  </si>
+  <si>
+    <t>Level</t>
   </si>
 </sst>
 </file>
@@ -979,7 +982,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,7 +998,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>25</v>

</xml_diff>